<commit_message>
add response rate table
</commit_message>
<xml_diff>
--- a/utils/excelTemplate/response_rate.xlsx
+++ b/utils/excelTemplate/response_rate.xlsx
@@ -1,36 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\jr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\jr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{63C830D9-C775-4CE2-A67C-98AA3C641347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7026E06F-9379-4E55-BDC7-D7F22A7A63E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recovered_Sheet1" sheetId="1" state="veryHidden" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="23" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="61">
   <si>
     <t>%</t>
   </si>
@@ -210,14 +201,17 @@
   </si>
   <si>
     <t>ปี 2566</t>
+  </si>
+  <si>
+    <t>ไตรมาส</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="194" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="187" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -442,11 +436,11 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="194" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="187" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="4" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -455,7 +449,7 @@
     <xf numFmtId="4" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -470,31 +464,28 @@
     <xf numFmtId="4" fontId="7" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -506,13 +497,13 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="194" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="187" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="194" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="187" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -527,28 +518,25 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="194" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="194" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="187" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="187" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="194" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="187" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -557,49 +545,49 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="187" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="187" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="187" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="187" fontId="6" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="187" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="187" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="187" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="187" fontId="6" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="187" fontId="6" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="187" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="194" fontId="6" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="194" fontId="6" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="194" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="194" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="194" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="194" fontId="6" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="194" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="194" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="194" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="194" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1836,7 +1824,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1"/>
   <sheetViews>
@@ -1852,11 +1840,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AD16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.9" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -1888,35 +1876,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="27.95" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="45"/>
-      <c r="S1" s="45"/>
-      <c r="T1" s="45"/>
-      <c r="U1" s="45"/>
-      <c r="V1" s="45"/>
-      <c r="W1" s="45"/>
-      <c r="X1" s="45"/>
-      <c r="Y1" s="45"/>
-      <c r="Z1" s="45"/>
-      <c r="AA1" s="45"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
+      <c r="S1" s="50"/>
+      <c r="T1" s="50"/>
+      <c r="U1" s="50"/>
+      <c r="V1" s="50"/>
+      <c r="W1" s="50"/>
+      <c r="X1" s="50"/>
+      <c r="Y1" s="50"/>
+      <c r="Z1" s="50"/>
+      <c r="AA1" s="50"/>
       <c r="AB1" s="10"/>
       <c r="AC1" s="10"/>
       <c r="AD1" s="10"/>
@@ -1996,385 +1984,382 @@
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16"/>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="16"/>
-      <c r="S4" s="16"/>
-      <c r="T4" s="16"/>
-      <c r="U4" s="16"/>
-      <c r="V4" s="16"/>
-      <c r="W4" s="16"/>
-      <c r="X4" s="17"/>
-      <c r="Y4" s="16"/>
-      <c r="Z4" s="16"/>
-      <c r="AA4" s="16"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="15"/>
+      <c r="T4" s="15"/>
+      <c r="U4" s="15"/>
+      <c r="V4" s="15"/>
+      <c r="W4" s="15"/>
+      <c r="X4" s="16"/>
+      <c r="Y4" s="15"/>
+      <c r="Z4" s="15"/>
+      <c r="AA4" s="15"/>
     </row>
     <row r="5" spans="1:30" s="13" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="18"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="20"/>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="20"/>
-      <c r="R5" s="20"/>
-      <c r="S5" s="20"/>
-      <c r="T5" s="20"/>
-      <c r="U5" s="20"/>
-      <c r="V5" s="20"/>
-      <c r="W5" s="20"/>
-      <c r="X5" s="20" t="s">
+      <c r="A5" s="17"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="19"/>
+      <c r="S5" s="19"/>
+      <c r="T5" s="19"/>
+      <c r="U5" s="19"/>
+      <c r="V5" s="19"/>
+      <c r="W5" s="19"/>
+      <c r="X5" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="Y5" s="20"/>
-      <c r="Z5" s="37"/>
-      <c r="AA5" s="20"/>
-      <c r="AB5" s="21"/>
-      <c r="AC5" s="21"/>
-      <c r="AD5" s="21"/>
+      <c r="Y5" s="19"/>
+      <c r="Z5" s="35"/>
+      <c r="AA5" s="19"/>
+      <c r="AB5" s="20"/>
+      <c r="AC5" s="20"/>
+      <c r="AD5" s="20"/>
     </row>
     <row r="6" spans="1:30" s="13" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="B6" s="38" t="s">
+      <c r="A6" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="40" t="s">
+      <c r="C6" s="47"/>
+      <c r="D6" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="40" t="s">
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="I6" s="41"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="41"/>
-      <c r="L6" s="41"/>
-      <c r="M6" s="41"/>
-      <c r="N6" s="41"/>
-      <c r="O6" s="41"/>
-      <c r="P6" s="41"/>
-      <c r="Q6" s="41"/>
-      <c r="R6" s="41"/>
-      <c r="S6" s="41"/>
-      <c r="T6" s="41"/>
-      <c r="U6" s="41"/>
-      <c r="V6" s="41"/>
-      <c r="W6" s="41"/>
-      <c r="X6" s="41"/>
-      <c r="Y6" s="41"/>
-      <c r="Z6" s="41"/>
-      <c r="AA6" s="42"/>
-      <c r="AB6" s="21"/>
-      <c r="AC6" s="21"/>
-      <c r="AD6" s="21"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="44"/>
+      <c r="M6" s="44"/>
+      <c r="N6" s="44"/>
+      <c r="O6" s="44"/>
+      <c r="P6" s="44"/>
+      <c r="Q6" s="44"/>
+      <c r="R6" s="44"/>
+      <c r="S6" s="44"/>
+      <c r="T6" s="44"/>
+      <c r="U6" s="44"/>
+      <c r="V6" s="44"/>
+      <c r="W6" s="44"/>
+      <c r="X6" s="44"/>
+      <c r="Y6" s="44"/>
+      <c r="Z6" s="44"/>
+      <c r="AA6" s="45"/>
+      <c r="AB6" s="20"/>
+      <c r="AC6" s="20"/>
+      <c r="AD6" s="20"/>
     </row>
     <row r="7" spans="1:30" s="13" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="24"/>
-      <c r="B7" s="43" t="s">
+      <c r="A7" s="23"/>
+      <c r="B7" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="46" t="s">
+      <c r="C7" s="49"/>
+      <c r="D7" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="47"/>
-      <c r="F7" s="46" t="s">
+      <c r="E7" s="37"/>
+      <c r="F7" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="47"/>
-      <c r="H7" s="46" t="s">
+      <c r="G7" s="37"/>
+      <c r="H7" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="47"/>
-      <c r="J7" s="46" t="s">
+      <c r="I7" s="37"/>
+      <c r="J7" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="47"/>
-      <c r="L7" s="46" t="s">
+      <c r="K7" s="37"/>
+      <c r="L7" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="47"/>
-      <c r="N7" s="46" t="s">
+      <c r="M7" s="37"/>
+      <c r="N7" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="O7" s="47"/>
-      <c r="P7" s="46" t="s">
+      <c r="O7" s="37"/>
+      <c r="P7" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="Q7" s="47"/>
-      <c r="R7" s="46" t="s">
+      <c r="Q7" s="37"/>
+      <c r="R7" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="S7" s="47"/>
-      <c r="T7" s="46" t="s">
+      <c r="S7" s="37"/>
+      <c r="T7" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="U7" s="47"/>
-      <c r="V7" s="46" t="s">
+      <c r="U7" s="37"/>
+      <c r="V7" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="W7" s="47"/>
-      <c r="X7" s="46" t="s">
+      <c r="W7" s="37"/>
+      <c r="X7" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="Y7" s="47"/>
-      <c r="Z7" s="46" t="s">
+      <c r="Y7" s="37"/>
+      <c r="Z7" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="AA7" s="47"/>
-      <c r="AB7" s="50"/>
-      <c r="AC7" s="50"/>
-      <c r="AD7" s="50"/>
+      <c r="AA7" s="37"/>
+      <c r="AB7" s="38"/>
+      <c r="AC7" s="38"/>
+      <c r="AD7" s="38"/>
     </row>
     <row r="8" spans="1:30" s="13" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="25"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="48" t="s">
+      <c r="A8" s="24"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="49"/>
-      <c r="F8" s="48" t="s">
+      <c r="E8" s="40"/>
+      <c r="F8" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="49"/>
-      <c r="H8" s="48" t="s">
+      <c r="G8" s="40"/>
+      <c r="H8" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="49"/>
-      <c r="J8" s="48" t="s">
+      <c r="I8" s="40"/>
+      <c r="J8" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="K8" s="49"/>
-      <c r="L8" s="48" t="s">
+      <c r="K8" s="40"/>
+      <c r="L8" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="M8" s="49"/>
-      <c r="N8" s="48" t="s">
+      <c r="M8" s="40"/>
+      <c r="N8" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="O8" s="49"/>
-      <c r="P8" s="51" t="s">
+      <c r="O8" s="40"/>
+      <c r="P8" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="Q8" s="52"/>
-      <c r="R8" s="48" t="s">
+      <c r="Q8" s="42"/>
+      <c r="R8" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="S8" s="49"/>
-      <c r="T8" s="48" t="s">
+      <c r="S8" s="40"/>
+      <c r="T8" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="U8" s="49"/>
-      <c r="V8" s="48" t="s">
+      <c r="U8" s="40"/>
+      <c r="V8" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="W8" s="49"/>
-      <c r="X8" s="48" t="s">
+      <c r="W8" s="40"/>
+      <c r="X8" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="Y8" s="49"/>
-      <c r="Z8" s="48" t="s">
+      <c r="Y8" s="40"/>
+      <c r="Z8" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="AA8" s="49"/>
-      <c r="AB8" s="21"/>
-      <c r="AC8" s="21"/>
-      <c r="AD8" s="21"/>
+      <c r="AA8" s="40"/>
+      <c r="AB8" s="20"/>
+      <c r="AC8" s="20"/>
+      <c r="AD8" s="20"/>
     </row>
     <row r="9" spans="1:30" s="13" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="27"/>
-      <c r="B9" s="23" t="s">
+      <c r="A9" s="26"/>
+      <c r="B9" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="29" t="s">
+      <c r="D9" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="29" t="s">
+      <c r="E9" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="F9" s="29" t="s">
+      <c r="F9" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="29" t="s">
+      <c r="G9" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="H9" s="29" t="s">
+      <c r="H9" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="29" t="s">
+      <c r="I9" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="J9" s="29" t="s">
+      <c r="J9" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="K9" s="29" t="s">
+      <c r="K9" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="L9" s="29" t="s">
+      <c r="L9" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="M9" s="29" t="s">
+      <c r="M9" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="N9" s="29" t="s">
+      <c r="N9" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="O9" s="29" t="s">
+      <c r="O9" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="P9" s="28" t="s">
+      <c r="P9" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="Q9" s="28" t="s">
+      <c r="Q9" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="R9" s="29" t="s">
+      <c r="R9" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="S9" s="29" t="s">
+      <c r="S9" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="T9" s="29" t="s">
+      <c r="T9" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="U9" s="29" t="s">
+      <c r="U9" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="V9" s="29" t="s">
+      <c r="V9" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="W9" s="29" t="s">
+      <c r="W9" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="X9" s="29" t="s">
+      <c r="X9" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="Y9" s="29" t="s">
+      <c r="Y9" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="Z9" s="29" t="s">
+      <c r="Z9" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="AA9" s="29" t="s">
+      <c r="AA9" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="AB9" s="21"/>
-      <c r="AC9" s="21"/>
-      <c r="AD9" s="21"/>
+      <c r="AB9" s="20"/>
+      <c r="AC9" s="20"/>
+      <c r="AD9" s="20"/>
     </row>
-    <row r="10" spans="1:30" s="32" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="30" t="s">
+    <row r="10" spans="1:30" s="30" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="30" t="s">
+      <c r="E10" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="30" t="s">
+      <c r="F10" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="G10" s="30" t="s">
+      <c r="G10" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="30" t="s">
+      <c r="H10" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="I10" s="30" t="s">
+      <c r="I10" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="J10" s="30" t="s">
+      <c r="J10" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="K10" s="30" t="s">
+      <c r="K10" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="L10" s="30" t="s">
+      <c r="L10" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="M10" s="30" t="s">
+      <c r="M10" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="N10" s="30" t="s">
+      <c r="N10" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="O10" s="30" t="s">
+      <c r="O10" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="P10" s="30" t="s">
+      <c r="P10" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="Q10" s="30" t="s">
+      <c r="Q10" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="R10" s="30" t="s">
+      <c r="R10" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="S10" s="30" t="s">
+      <c r="S10" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="T10" s="30" t="s">
+      <c r="T10" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="U10" s="30" t="s">
+      <c r="U10" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="V10" s="30" t="s">
+      <c r="V10" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="W10" s="30" t="s">
+      <c r="W10" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="X10" s="30" t="s">
+      <c r="X10" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="Y10" s="30" t="s">
+      <c r="Y10" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="Z10" s="30" t="s">
+      <c r="Z10" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="AA10" s="30" t="s">
+      <c r="AA10" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="AB10" s="31"/>
-      <c r="AC10" s="31"/>
-      <c r="AD10" s="31"/>
     </row>
     <row r="11" spans="1:30" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="24"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -2401,12 +2386,12 @@
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
-      <c r="AB11" s="33"/>
-      <c r="AC11" s="33"/>
-      <c r="AD11" s="33"/>
+      <c r="AB11" s="31"/>
+      <c r="AC11" s="31"/>
+      <c r="AD11" s="31"/>
     </row>
     <row r="12" spans="1:30" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="24"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="1"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -2433,12 +2418,12 @@
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
       <c r="AA12" s="2"/>
-      <c r="AB12" s="34"/>
-      <c r="AC12" s="34"/>
-      <c r="AD12" s="34"/>
+      <c r="AB12" s="32"/>
+      <c r="AC12" s="32"/>
+      <c r="AD12" s="32"/>
     </row>
     <row r="13" spans="1:30" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="24"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="3"/>
@@ -2465,12 +2450,12 @@
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
       <c r="AA13" s="2"/>
-      <c r="AB13" s="33"/>
-      <c r="AC13" s="33"/>
-      <c r="AD13" s="33"/>
+      <c r="AB13" s="31"/>
+      <c r="AC13" s="31"/>
+      <c r="AD13" s="31"/>
     </row>
     <row r="14" spans="1:30" ht="22.9" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="27"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="5"/>
@@ -2497,15 +2482,34 @@
       <c r="Y14" s="7"/>
       <c r="Z14" s="7"/>
       <c r="AA14" s="8"/>
-      <c r="AB14" s="35"/>
-      <c r="AC14" s="35"/>
-      <c r="AD14" s="35"/>
+      <c r="AB14" s="33"/>
+      <c r="AC14" s="33"/>
+      <c r="AD14" s="33"/>
     </row>
     <row r="16" spans="1:30" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="AA16" s="36"/>
+      <c r="AA16" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="A1:AA1"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="H6:AA6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="Z7:AA7"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="T7:U7"/>
+    <mergeCell ref="T8:U8"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="V8:W8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="N8:O8"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="V7:W7"/>
     <mergeCell ref="AB7:AD7"/>
@@ -2517,25 +2521,6 @@
     <mergeCell ref="N7:O7"/>
     <mergeCell ref="P8:Q8"/>
     <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H6:AA6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="Z7:AA7"/>
-    <mergeCell ref="R8:S8"/>
-    <mergeCell ref="T7:U7"/>
-    <mergeCell ref="T8:U8"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="A1:AA1"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="V8:W8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="J7:K7"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>